<commit_message>
EPBDS-9097 Rewrite one test case for exp() function to pass under Java 11.
Oracle replaced implementation of java Math in Java 11 which has other calculation accuracy.
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Math.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Math.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\DEV\org.openl.test\test\rules\functionality\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="285" yWindow="105" windowWidth="16140" windowHeight="9210" tabRatio="765" activeTab="8"/>
+    <workbookView xWindow="285" yWindow="105" windowWidth="16140" windowHeight="9210" tabRatio="765" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="X" sheetId="5" r:id="rId1"/>
@@ -31,7 +26,7 @@
     <sheet name="nextAfter" sheetId="22" r:id="rId17"/>
     <sheet name="random" sheetId="44" r:id="rId18"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -41,7 +36,7 @@
     <author>Polina Kaziuchyts</author>
   </authors>
   <commentList>
-    <comment ref="C13" authorId="0" shapeId="0">
+    <comment ref="C13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -68,7 +63,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C80" authorId="0" shapeId="0">
+    <comment ref="C80" authorId="0">
       <text>
         <r>
           <rPr>
@@ -94,7 +89,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E85" authorId="0" shapeId="0">
+    <comment ref="E85" authorId="0">
       <text>
         <r>
           <rPr>
@@ -121,7 +116,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E101" authorId="0" shapeId="0">
+    <comment ref="E101" authorId="0">
       <text>
         <r>
           <rPr>
@@ -157,7 +152,7 @@
     <author>Polina Kaziuchyts</author>
   </authors>
   <commentList>
-    <comment ref="D50" authorId="0" shapeId="0">
+    <comment ref="D50" authorId="0">
       <text>
         <r>
           <rPr>
@@ -244,7 +239,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D51" authorId="0" shapeId="0">
+    <comment ref="D51" authorId="0">
       <text>
         <r>
           <rPr>
@@ -346,7 +341,7 @@
     <author>Polina Kaziuchyts</author>
   </authors>
   <commentList>
-    <comment ref="B3" authorId="0" shapeId="0">
+    <comment ref="B3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -370,7 +365,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D11" authorId="0" shapeId="0">
+    <comment ref="D11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -394,7 +389,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D12" authorId="0" shapeId="0">
+    <comment ref="D12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -418,7 +413,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D19" authorId="0" shapeId="0">
+    <comment ref="D19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -442,7 +437,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D20" authorId="0" shapeId="0">
+    <comment ref="D20" authorId="0">
       <text>
         <r>
           <rPr>
@@ -466,7 +461,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D41" authorId="0" shapeId="0">
+    <comment ref="D41" authorId="0">
       <text>
         <r>
           <rPr>
@@ -490,7 +485,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D42" authorId="0" shapeId="0">
+    <comment ref="D42" authorId="0">
       <text>
         <r>
           <rPr>
@@ -514,7 +509,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D43" authorId="0" shapeId="0">
+    <comment ref="D43" authorId="0">
       <text>
         <r>
           <rPr>
@@ -538,7 +533,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D44" authorId="0" shapeId="0">
+    <comment ref="D44" authorId="0">
       <text>
         <r>
           <rPr>
@@ -567,7 +562,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="319">
   <si>
     <t>_res_</t>
   </si>
@@ -1106,9 +1101,6 @@
     <t>0.010050167084168058</t>
   </si>
   <si>
-    <t>5.968551312745626E156</t>
-  </si>
-  <si>
     <t>2.2405592344158094E156</t>
   </si>
   <si>
@@ -1521,12 +1513,18 @@
   </si>
   <si>
     <t>Method String formatMethod_formatter (Double a, String fmt)</t>
+  </si>
+  <si>
+    <t>360.98977874</t>
+  </si>
+  <si>
+    <t>5.9685512897846565E156</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="8">
     <numFmt numFmtId="164" formatCode="0.0000000000000000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -1913,7 +1911,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2715,31 +2713,31 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" s="72" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C2" s="72"/>
       <c r="D2" s="72"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B3" s="73" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C3" s="73"/>
       <c r="D3" s="73"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" s="70" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C5" s="74"/>
       <c r="D5" s="71"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="30" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
@@ -2747,10 +2745,10 @@
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" s="28" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D7" s="28" t="s">
         <v>1</v>
@@ -2813,7 +2811,7 @@
         <v>8</v>
       </c>
       <c r="D13" s="65" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.2">
@@ -2840,13 +2838,13 @@
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B16" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C16" s="43">
         <v>8</v>
       </c>
       <c r="D16" s="62" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
@@ -2857,7 +2855,7 @@
         <v>-8</v>
       </c>
       <c r="D17" s="62" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
@@ -2896,31 +2894,31 @@
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25" s="72" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C25" s="72"/>
       <c r="D25" s="72"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="73" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C26" s="73"/>
       <c r="D26" s="73"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="70" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C28" s="74"/>
       <c r="D28" s="71"/>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B29" s="30" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C29" s="30" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D29" s="31" t="s">
         <v>0</v>
@@ -2928,10 +2926,10 @@
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B30" s="28" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C30" s="28" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D30" s="28" t="s">
         <v>1</v>
@@ -2994,7 +2992,7 @@
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C36" s="43">
         <v>8</v>
@@ -3581,19 +3579,19 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B2" s="72" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C2" s="72"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="73" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C3" s="73"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="70" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C5" s="71"/>
     </row>
@@ -3937,31 +3935,31 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" s="72" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C2" s="72"/>
       <c r="D2" s="72"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B3" s="73" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C3" s="73"/>
       <c r="D3" s="73"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" s="70" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C5" s="74"/>
       <c r="D5" s="71"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="30" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D6" s="27" t="s">
         <v>0</v>
@@ -3969,10 +3967,10 @@
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" s="28" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D7" s="34" t="s">
         <v>1</v>
@@ -4181,7 +4179,7 @@
         <v>1</v>
       </c>
       <c r="C26" s="26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D26" s="35" t="s">
         <v>26</v>
@@ -4192,7 +4190,7 @@
         <v>180</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D27" s="35" t="s">
         <v>96</v>
@@ -4203,7 +4201,7 @@
         <v>-180</v>
       </c>
       <c r="C28" s="26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>96</v>
@@ -4214,10 +4212,10 @@
         <v>58</v>
       </c>
       <c r="C29" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="D29" s="14" t="s">
         <v>194</v>
-      </c>
-      <c r="D29" s="14" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
@@ -4225,10 +4223,10 @@
         <v>0</v>
       </c>
       <c r="C30" s="26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.2">
@@ -4236,10 +4234,10 @@
         <v>0.01</v>
       </c>
       <c r="C31" s="26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
@@ -4247,10 +4245,10 @@
         <v>34</v>
       </c>
       <c r="C32" s="26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
@@ -4258,7 +4256,7 @@
         <v>360.01</v>
       </c>
       <c r="C33" s="26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>47</v>
@@ -4269,7 +4267,7 @@
         <v>47</v>
       </c>
       <c r="C34" s="26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>47</v>
@@ -4277,31 +4275,31 @@
     </row>
     <row r="37" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="72" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C37" s="72"/>
       <c r="D37" s="72"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" s="73" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C38" s="73"/>
       <c r="D38" s="73"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B40" s="70" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C40" s="74"/>
       <c r="D40" s="71"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B41" s="30" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C41" s="30" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D41" s="27" t="s">
         <v>0</v>
@@ -4309,10 +4307,10 @@
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B42" s="28" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C42" s="28" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D42" s="34" t="s">
         <v>1</v>
@@ -4521,7 +4519,7 @@
         <v>1</v>
       </c>
       <c r="C61" s="26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D61" s="35" t="s">
         <v>26</v>
@@ -4532,7 +4530,7 @@
         <v>180</v>
       </c>
       <c r="C62" s="26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D62" s="35" t="s">
         <v>96</v>
@@ -4543,7 +4541,7 @@
         <v>-180</v>
       </c>
       <c r="C63" s="26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D63" s="14" t="s">
         <v>96</v>
@@ -4554,10 +4552,10 @@
         <v>58</v>
       </c>
       <c r="C64" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="D64" s="14" t="s">
         <v>194</v>
-      </c>
-      <c r="D64" s="14" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.2">
@@ -4565,10 +4563,10 @@
         <v>0</v>
       </c>
       <c r="C65" s="26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.2">
@@ -4576,10 +4574,10 @@
         <v>0.01</v>
       </c>
       <c r="C66" s="26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D66" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.2">
@@ -4587,10 +4585,10 @@
         <v>34</v>
       </c>
       <c r="C67" s="26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D67" s="14" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.2">
@@ -4598,7 +4596,7 @@
         <v>360.01</v>
       </c>
       <c r="C68" s="26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D68" s="14" t="s">
         <v>47</v>
@@ -4609,7 +4607,7 @@
         <v>47</v>
       </c>
       <c r="C69" s="26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D69" s="14" t="s">
         <v>47</v>
@@ -5126,31 +5124,31 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" s="72" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C2" s="72"/>
       <c r="D2" s="72"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B3" s="73" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C3" s="73"/>
       <c r="D3" s="73"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" s="70" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C5" s="74"/>
       <c r="D5" s="71"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="C6" s="30" t="s">
         <v>221</v>
-      </c>
-      <c r="C6" s="30" t="s">
-        <v>222</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
@@ -5158,10 +5156,10 @@
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" s="28" t="s">
+        <v>220</v>
+      </c>
+      <c r="C7" s="28" t="s">
         <v>221</v>
-      </c>
-      <c r="C7" s="28" t="s">
-        <v>222</v>
       </c>
       <c r="D7" s="28" t="s">
         <v>1</v>
@@ -5208,7 +5206,7 @@
         <v>59</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
@@ -5241,7 +5239,7 @@
         <v>59</v>
       </c>
       <c r="D14" s="49" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.2">
@@ -5370,7 +5368,7 @@
         <v>1</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D26" s="50">
         <v>-0.125</v>
@@ -5381,7 +5379,7 @@
         <v>180</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D27" s="50">
         <v>0</v>
@@ -5392,7 +5390,7 @@
         <v>-180</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D28" s="50">
         <v>0</v>
@@ -5403,7 +5401,7 @@
         <v>58</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D29" s="50">
         <v>-0.125</v>
@@ -5414,7 +5412,7 @@
         <v>0</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D30" s="50">
         <v>0</v>
@@ -5425,7 +5423,7 @@
         <v>0.01</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D31" s="50">
         <v>0.01</v>
@@ -5436,10 +5434,10 @@
         <v>34</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D32" s="51" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
@@ -5447,10 +5445,10 @@
         <v>360.01</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D33" s="51" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
@@ -5458,10 +5456,10 @@
         <v>47</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D34" s="51" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -6198,17 +6196,17 @@
   <sheetData>
     <row r="3" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B3" s="64" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B9" s="64" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.2">
@@ -6244,19 +6242,19 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B2" s="72" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C2" s="72"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="73" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C3" s="73"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="70" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C5" s="71"/>
     </row>
@@ -6281,7 +6279,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="38" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D8" s="39"/>
     </row>
@@ -6354,19 +6352,19 @@
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" s="72" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C20" s="72"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" s="73" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C21" s="73"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" s="70" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C23" s="71"/>
     </row>
@@ -6426,7 +6424,7 @@
         <v>0</v>
       </c>
       <c r="C30" s="38" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.2">
@@ -6434,7 +6432,7 @@
         <v>0.47942553860420301</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.2">
@@ -6463,19 +6461,19 @@
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B38" s="72" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C38" s="72"/>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B39" s="73" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C39" s="73"/>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B41" s="70" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C41" s="71"/>
     </row>
@@ -6500,7 +6498,7 @@
         <v>1</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.2">
@@ -6508,7 +6506,7 @@
         <v>180</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.2">
@@ -6516,7 +6514,7 @@
         <v>-180</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.2">
@@ -6524,7 +6522,7 @@
         <v>58</v>
       </c>
       <c r="C47" s="20" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.2">
@@ -6532,7 +6530,7 @@
         <v>0</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.2">
@@ -6540,7 +6538,7 @@
         <v>0.01</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.2">
@@ -6548,7 +6546,7 @@
         <v>34</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.2">
@@ -6556,7 +6554,7 @@
         <v>360.01</v>
       </c>
       <c r="C51" s="20" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.2">
@@ -6564,36 +6562,36 @@
         <v>47</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B56" s="72" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C56" s="72"/>
       <c r="D56" s="72"/>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B57" s="73" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C57" s="73"/>
       <c r="D57" s="73"/>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B59" s="70" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C59" s="74"/>
       <c r="D59" s="71"/>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B60" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="C60" s="30" t="s">
         <v>221</v>
-      </c>
-      <c r="C60" s="30" t="s">
-        <v>222</v>
       </c>
       <c r="D60" s="31" t="s">
         <v>0</v>
@@ -6601,10 +6599,10 @@
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B61" s="28" t="s">
+        <v>220</v>
+      </c>
+      <c r="C61" s="28" t="s">
         <v>221</v>
-      </c>
-      <c r="C61" s="28" t="s">
-        <v>222</v>
       </c>
       <c r="D61" s="28" t="s">
         <v>1</v>
@@ -6618,7 +6616,7 @@
         <v>59</v>
       </c>
       <c r="D62" s="20" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.2">
@@ -6629,7 +6627,7 @@
         <v>59</v>
       </c>
       <c r="D63" s="20" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.2">
@@ -6640,7 +6638,7 @@
         <v>59</v>
       </c>
       <c r="D64" s="20" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.2">
@@ -6651,7 +6649,7 @@
         <v>59</v>
       </c>
       <c r="D65" s="20" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.2">
@@ -6662,7 +6660,7 @@
         <v>59</v>
       </c>
       <c r="D66" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.2">
@@ -6673,7 +6671,7 @@
         <v>59</v>
       </c>
       <c r="D67" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.2">
@@ -6684,7 +6682,7 @@
         <v>59</v>
       </c>
       <c r="D68" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.2">
@@ -6695,7 +6693,7 @@
         <v>59</v>
       </c>
       <c r="D69" s="21" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.2">
@@ -6706,7 +6704,7 @@
         <v>59</v>
       </c>
       <c r="D70" s="21" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.2">
@@ -6717,7 +6715,7 @@
         <v>24</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.2">
@@ -6728,7 +6726,7 @@
         <v>24</v>
       </c>
       <c r="D72" s="14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.2">
@@ -6739,7 +6737,7 @@
         <v>24</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.2">
@@ -6750,7 +6748,7 @@
         <v>24</v>
       </c>
       <c r="D74" s="14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.2">
@@ -6772,7 +6770,7 @@
         <v>24</v>
       </c>
       <c r="D76" s="14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.2">
@@ -6783,7 +6781,7 @@
         <v>24</v>
       </c>
       <c r="D77" s="14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.2">
@@ -6794,7 +6792,7 @@
         <v>24</v>
       </c>
       <c r="D78" s="21" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.2">
@@ -6805,7 +6803,7 @@
         <v>24</v>
       </c>
       <c r="D79" s="19" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.2">
@@ -6813,10 +6811,10 @@
         <v>1</v>
       </c>
       <c r="C80" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D80" s="14" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.2">
@@ -6824,10 +6822,10 @@
         <v>180</v>
       </c>
       <c r="C81" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D81" s="14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.2">
@@ -6835,10 +6833,10 @@
         <v>-180</v>
       </c>
       <c r="C82" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D82" s="14" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.2">
@@ -6846,10 +6844,10 @@
         <v>58</v>
       </c>
       <c r="C83" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D83" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.2">
@@ -6857,10 +6855,10 @@
         <v>0</v>
       </c>
       <c r="C84" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D84" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.2">
@@ -6868,10 +6866,10 @@
         <v>0.01</v>
       </c>
       <c r="C85" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D85" s="14" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.2">
@@ -6879,10 +6877,10 @@
         <v>34</v>
       </c>
       <c r="C86" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D86" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.2">
@@ -6890,10 +6888,10 @@
         <v>360.01</v>
       </c>
       <c r="C87" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D87" s="19" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.2">
@@ -6901,10 +6899,10 @@
         <v>47</v>
       </c>
       <c r="C88" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D88" s="19" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -7525,8 +7523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7538,19 +7536,19 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" s="72" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C2" s="72"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="73" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C3" s="73"/>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="70" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C5" s="71"/>
     </row>
@@ -7575,7 +7573,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.2">
@@ -7591,7 +7589,7 @@
         <v>-180</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.2">
@@ -7615,15 +7613,15 @@
         <v>0.01</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B14" s="19" t="s">
-        <v>34</v>
+        <v>317</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>179</v>
+        <v>318</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.2">
@@ -7631,7 +7629,7 @@
         <v>360.01</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.2">
@@ -7639,7 +7637,7 @@
         <v>47</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.2">
@@ -7727,10 +7725,10 @@
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B32" s="19" t="s">
-        <v>34</v>
+        <v>317</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>179</v>
+        <v>318</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.2">
@@ -7738,7 +7736,7 @@
         <v>360.01</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.2">
@@ -8234,19 +8232,19 @@
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" s="72" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C20" s="72"/>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" s="73" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C21" s="73"/>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" s="70" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C23" s="71"/>
     </row>
@@ -8279,7 +8277,7 @@
         <v>180</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.2">
@@ -8287,7 +8285,7 @@
         <v>-180</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.2">
@@ -8295,7 +8293,7 @@
         <v>361</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.2">
@@ -8303,7 +8301,7 @@
         <v>0</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.2">
@@ -8311,7 +8309,7 @@
         <v>0.01</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.2">
@@ -8319,7 +8317,7 @@
         <v>360.98977874384701</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
@@ -8327,7 +8325,7 @@
         <v>360.01</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
@@ -8335,7 +8333,7 @@
         <v>-360.01</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
@@ -8711,19 +8709,19 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" s="72" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C2" s="72"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="73" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C3" s="73"/>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="70" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C5" s="71"/>
     </row>
@@ -9029,19 +9027,19 @@
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B56" s="72" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C56" s="72"/>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B57" s="73" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C57" s="73"/>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B59" s="70" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C59" s="71"/>
     </row>
@@ -9074,7 +9072,7 @@
         <v>180</v>
       </c>
       <c r="C63" s="14" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.2">
@@ -9082,7 +9080,7 @@
         <v>-180</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.2">
@@ -9090,7 +9088,7 @@
         <v>58</v>
       </c>
       <c r="C65" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.2">
@@ -9098,7 +9096,7 @@
         <v>0</v>
       </c>
       <c r="C66" s="14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.2">
@@ -9114,7 +9112,7 @@
         <v>34</v>
       </c>
       <c r="C68" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.2">
@@ -9122,7 +9120,7 @@
         <v>360.01</v>
       </c>
       <c r="C69" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.2">
@@ -9130,12 +9128,12 @@
         <v>47</v>
       </c>
       <c r="C70" s="14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B74" s="72" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C74" s="72"/>
       <c r="D74" s="72"/>
@@ -9143,7 +9141,7 @@
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B75" s="73" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C75" s="73"/>
       <c r="D75" s="73"/>
@@ -9151,7 +9149,7 @@
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B77" s="70" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C77" s="74"/>
       <c r="D77" s="74"/>
@@ -9162,10 +9160,10 @@
         <v>5</v>
       </c>
       <c r="C78" s="29" t="s">
+        <v>276</v>
+      </c>
+      <c r="D78" s="29" t="s">
         <v>277</v>
-      </c>
-      <c r="D78" s="29" t="s">
-        <v>278</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>0</v>
@@ -9176,10 +9174,10 @@
         <v>5</v>
       </c>
       <c r="C79" s="33" t="s">
+        <v>276</v>
+      </c>
+      <c r="D79" s="33" t="s">
         <v>277</v>
-      </c>
-      <c r="D79" s="33" t="s">
-        <v>278</v>
       </c>
       <c r="E79" s="18" t="s">
         <v>1</v>
@@ -9479,21 +9477,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B56:C56"/>
     <mergeCell ref="B57:C57"/>
     <mergeCell ref="B59:C59"/>
     <mergeCell ref="B74:E74"/>
     <mergeCell ref="B75:E75"/>
     <mergeCell ref="B77:E77"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -9504,7 +9502,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -9517,19 +9515,19 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" s="72" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C2" s="72"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="73" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C3" s="73"/>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="70" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C5" s="71"/>
     </row>
@@ -9623,14 +9621,14 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="72" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C20" s="72"/>
       <c r="D20" s="72"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" s="73" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C21" s="73"/>
       <c r="D21" s="73"/>
@@ -9647,7 +9645,7 @@
         <v>5</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>0</v>
@@ -9658,7 +9656,7 @@
         <v>5</v>
       </c>
       <c r="C25" s="33" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D25" s="18" t="s">
         <v>1</v>
@@ -9768,10 +9766,10 @@
         <v>1</v>
       </c>
       <c r="C35" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="D35" s="14" t="s">
         <v>294</v>
-      </c>
-      <c r="D35" s="14" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
@@ -9779,10 +9777,10 @@
         <v>180</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
@@ -9790,10 +9788,10 @@
         <v>-180</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D37" s="14" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
@@ -9801,10 +9799,10 @@
         <v>58</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D38" s="14" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
@@ -9812,10 +9810,10 @@
         <v>0</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D39" s="14" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
@@ -9823,10 +9821,10 @@
         <v>0.01</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.2">
@@ -9834,10 +9832,10 @@
         <v>34</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.2">
@@ -9845,10 +9843,10 @@
         <v>360.01</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.2">
@@ -9856,10 +9854,10 @@
         <v>47</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.2">
@@ -9867,10 +9865,10 @@
         <v>1</v>
       </c>
       <c r="C44" s="14" t="s">
+        <v>303</v>
+      </c>
+      <c r="D44" s="14" t="s">
         <v>304</v>
-      </c>
-      <c r="D44" s="14" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.2">
@@ -9878,10 +9876,10 @@
         <v>180</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.2">
@@ -9889,10 +9887,10 @@
         <v>-180</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.2">
@@ -9900,10 +9898,10 @@
         <v>58</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.2">
@@ -9911,10 +9909,10 @@
         <v>0</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.2">
@@ -9922,10 +9920,10 @@
         <v>0.01</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D49" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.2">
@@ -9933,10 +9931,10 @@
         <v>34</v>
       </c>
       <c r="C50" s="63" t="s">
+        <v>311</v>
+      </c>
+      <c r="D50" s="63" t="s">
         <v>312</v>
-      </c>
-      <c r="D50" s="63" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.2">
@@ -9944,10 +9942,10 @@
         <v>34</v>
       </c>
       <c r="C51" s="63" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D51" s="63" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.2">
@@ -9955,10 +9953,10 @@
         <v>360.01</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D52" s="14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.2">
@@ -9966,10 +9964,10 @@
         <v>47</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D53" s="14" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>

</xml_diff>